<commit_message>
error catch and excel file uploading
</commit_message>
<xml_diff>
--- a/Sample_4.xlsx
+++ b/Sample_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hangliu/sei-course/final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F564E8-CC48-A64D-B369-59746BBD2032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191F8F7C-177B-9C47-872D-F139CFE32235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6CC3BDB0-75B4-B64E-B53C-367D30883A9C}"/>
+    <workbookView xWindow="33720" yWindow="3940" windowWidth="28040" windowHeight="16380" xr2:uid="{6CC3BDB0-75B4-B64E-B53C-367D30883A9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>carrier</t>
   </si>
@@ -62,25 +62,40 @@
     <t>Qantas</t>
   </si>
   <si>
-    <t>Jakarta</t>
-  </si>
-  <si>
-    <t>Sydney</t>
-  </si>
-  <si>
     <t>Singapore Airline</t>
   </si>
   <si>
     <t>Bangkok</t>
   </si>
   <si>
-    <t>Brisbane</t>
-  </si>
-  <si>
-    <t>ANA</t>
-  </si>
-  <si>
-    <t>Tokyo</t>
+    <t>Melbourne</t>
+  </si>
+  <si>
+    <t>Malaysian Air</t>
+  </si>
+  <si>
+    <t>Kuala Lumpur</t>
+  </si>
+  <si>
+    <t>Perth</t>
+  </si>
+  <si>
+    <t>Air China</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>Delta Air</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Adelaide</t>
   </si>
 </sst>
 </file>
@@ -90,8 +105,16 @@
   <numFmts count="1">
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -119,12 +142,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,7 +466,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,25 +477,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -480,75 +504,115 @@
         <v>7</v>
       </c>
       <c r="B2" s="1">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="C2" s="1">
-        <v>10.199999999999999</v>
+        <v>11.5</v>
       </c>
       <c r="D2" s="1">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" s="4">
-        <v>45000</v>
+        <v>45014</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C3" s="1">
-        <v>10.199999999999999</v>
+        <v>10.8</v>
       </c>
       <c r="D3" s="1">
-        <v>0.93</v>
+        <v>1.05</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="4">
-        <v>45007</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>155</v>
+      </c>
+      <c r="C4">
+        <v>11.2</v>
+      </c>
+      <c r="D4">
+        <v>1.25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4">
+        <v>45017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>175</v>
+      </c>
+      <c r="C5">
+        <v>10.5</v>
+      </c>
+      <c r="D5">
+        <v>1.05</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="4">
+        <v>45046</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>145</v>
+      </c>
+      <c r="C6">
+        <v>9.5</v>
+      </c>
+      <c r="D6">
+        <v>1.25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
-        <v>129</v>
-      </c>
-      <c r="C4">
-        <v>10.3</v>
-      </c>
-      <c r="D4">
-        <v>0.89</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="3">
-        <v>45004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G6" s="3"/>
+      <c r="G6" s="4">
+        <v>45031</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G7" s="3"/>

</xml_diff>